<commit_message>
made n_same_system_parallel run for higher values of n by combining like terms on every iteration, requiring much smaller arrays finalized distribution for DC system with passive balancing: X4, P4. (includes PB systems, DC/DC converters, and inverters
</commit_message>
<xml_diff>
--- a/failurerates_v1.xlsx
+++ b/failurerates_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arossic/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alina/Documents/NREL/reliability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2369AA31-C6EC-4F49-91A4-1C36684CEBA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A1E5E5-6270-D349-A20A-434F3FA7A40D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{7A757A32-EF60-5542-B59E-9AF6649078C5}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{7A757A32-EF60-5542-B59E-9AF6649078C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Component</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>resistor</t>
+  </si>
+  <si>
+    <t>Passive balancing</t>
+  </si>
+  <si>
+    <t>system</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD266A6-BE7D-8E47-ADD4-1A022451240B}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +679,7 @@
         <v>96000</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M3:M6" si="4">EXP(-K4*L4)</f>
+        <f t="shared" ref="M4:M6" si="4">EXP(-K4*L4)</f>
         <v>0.9967196003069172</v>
       </c>
       <c r="N4" s="2">
@@ -912,7 +918,141 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1.5790000000000001E-3</v>
+      </c>
+      <c r="D19">
+        <f>C19/10^6</f>
+        <v>1.579E-9</v>
+      </c>
+      <c r="E19">
+        <v>96000</v>
+      </c>
+      <c r="F19" s="1">
+        <f>EXP(-D19*E19)</f>
+        <v>0.99984842748827407</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1.5661999999999999E-2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D24" si="5">C20/10^6</f>
+        <v>1.5661999999999998E-8</v>
+      </c>
+      <c r="E20">
+        <v>96000</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" ref="F20:F22" si="6">EXP(-D20*E20)</f>
+        <v>0.99849757776801573</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>7.5132000000000004E-2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="5"/>
+        <v>7.5132000000000001E-8</v>
+      </c>
+      <c r="E21">
+        <v>96000</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.99281327689425547</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>2.64E-3</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="5"/>
+        <v>2.64E-9</v>
+      </c>
+      <c r="E22">
+        <v>96000</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="6"/>
+        <v>0.99974659211320382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" cm="1">
+        <f t="array" ref="C24">SUM(B19:B22*C19:C22)</f>
+        <v>0.10029300000000001</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="5"/>
+        <v>1.0029300000000001E-7</v>
+      </c>
+      <c r="E24">
+        <v>96000</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" ref="F24" si="7">EXP(-D24*E24)</f>
+        <v>0.99041807402582449</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
checked base failure rates, modified table
</commit_message>
<xml_diff>
--- a/failurerates_v1.xlsx
+++ b/failurerates_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alina/Documents/NREL/reliability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A1E5E5-6270-D349-A20A-434F3FA7A40D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41425249-261A-7C4D-9BB8-77695010B28F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{7A757A32-EF60-5542-B59E-9AF6649078C5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{7A757A32-EF60-5542-B59E-9AF6649078C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -497,7 +497,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,6 +507,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -603,18 +604,18 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1.5661999999999999E-2</v>
+        <v>1.9650000000000002E-3</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D6" si="1">C3/10^6</f>
-        <v>1.5661999999999998E-8</v>
+        <v>1.9650000000000001E-9</v>
       </c>
       <c r="E3">
         <v>96000</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F6" si="2">EXP(-D3*E3)</f>
-        <v>0.99849757776801573</v>
+        <v>0.99981137779140605</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -623,22 +624,23 @@
         <v>6</v>
       </c>
       <c r="J3">
-        <v>1.5661999999999999E-2</v>
+        <f>C3</f>
+        <v>1.9650000000000002E-3</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>1.5661999999999998E-8</v>
+        <v>1.9650000000000001E-9</v>
       </c>
       <c r="L3">
         <v>96000</v>
       </c>
       <c r="M3" s="1">
         <f>EXP(-K3*L3)</f>
-        <v>0.99849757776801573</v>
+        <v>0.99981137779140605</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" ref="N3:N6" si="3">M3^I3</f>
-        <v>0.99101925794539558</v>
+        <v>0.99886880028930181</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -649,18 +651,18 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>7.5132000000000004E-2</v>
+        <v>1.7840000000000002E-2</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>7.5132000000000001E-8</v>
+        <v>1.7840000000000003E-8</v>
       </c>
       <c r="E4">
         <v>96000</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="2"/>
-        <v>0.99281327689425547</v>
+        <v>0.99828882573100886</v>
       </c>
       <c r="H4" t="s">
         <v>23</v>
@@ -669,22 +671,22 @@
         <v>6</v>
       </c>
       <c r="J4">
-        <v>3.4227E-2</v>
+        <v>1.5855000000000001E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>3.4226999999999999E-8</v>
+        <v>1.5855000000000002E-8</v>
       </c>
       <c r="L4">
         <v>96000</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" ref="M4:M6" si="4">EXP(-K4*L4)</f>
-        <v>0.9967196003069172</v>
+        <v>0.99847907777627931</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="3"/>
-        <v>0.98047831289933995</v>
+        <v>0.99090909443996988</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -782,7 +784,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N7" s="2">
         <f>PRODUCT(N2:N6)</f>
-        <v>0.96945850859473093</v>
+        <v>0.98753251326850944</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -791,11 +793,15 @@
       </c>
       <c r="B8">
         <f>(F2)^2*(F3*F4)^8*F5*F6</f>
-        <v>0.92566199393483162</v>
+        <v>0.97752972701156593</v>
       </c>
       <c r="C8">
-        <f>2*D2+8*(D3+D4)+D5+D6</f>
-        <v>8.0464717E-7</v>
+        <f>B2*D2+B3*(D3+D4)+D5+D6</f>
+        <v>2.3673517000000004E-7</v>
+      </c>
+      <c r="D8">
+        <f>C8*10^6</f>
+        <v>0.23673517000000005</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -814,9 +820,13 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f>EXP(-C8*0.2*E4)</f>
+        <v>0.99546499904824015</v>
+      </c>
       <c r="C9">
         <f>EXP(-C8*E6)</f>
-        <v>0.92566199393483151</v>
+        <v>0.97752972701156615</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -831,23 +841,31 @@
       </c>
       <c r="I9" cm="1">
         <f t="array" ref="I9">PRODUCT(M2:M6^I2:I6)</f>
-        <v>0.96945850859473093</v>
+        <v>0.98753251326850944</v>
       </c>
       <c r="J9" cm="1">
         <f t="array" ref="J9">SUM(I2:I6*K2:K6)</f>
-        <v>3.2310001999999994E-7</v>
+        <v>1.3068602000000003E-7</v>
       </c>
       <c r="K9">
         <f>EXP(-J9*L6)</f>
-        <v>0.96945850859473093</v>
+        <v>0.98753251326850955</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
+      <c r="C10">
+        <f>EXP(-C8*E6*0.2)</f>
+        <v>0.99546499904824015</v>
+      </c>
       <c r="D10" t="s">
         <v>20</v>
+      </c>
+      <c r="J10">
+        <f>J9*10^6</f>
+        <v>0.13068602000000004</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -879,11 +897,11 @@
       </c>
       <c r="E12">
         <f>B8</f>
-        <v>0.92566199393483162</v>
+        <v>0.97752972701156593</v>
       </c>
       <c r="J12">
         <f>I2*J2+6*SUM(J3:J6)</f>
-        <v>0.32310002000000004</v>
+        <v>0.13068602000000001</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -899,7 +917,7 @@
       </c>
       <c r="E13">
         <f>E12*E11^14</f>
-        <v>0.82709920154484884</v>
+        <v>0.87344415347632942</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -973,18 +991,18 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1.5661999999999999E-2</v>
+        <v>3.9659999999999999E-3</v>
       </c>
       <c r="D20">
         <f t="shared" ref="D20:D24" si="5">C20/10^6</f>
-        <v>1.5661999999999998E-8</v>
+        <v>3.9659999999999997E-9</v>
       </c>
       <c r="E20">
         <v>96000</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" ref="F20:F22" si="6">EXP(-D20*E20)</f>
-        <v>0.99849757776801573</v>
+        <v>0.99961933647075318</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -995,18 +1013,19 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>7.5132000000000004E-2</v>
+        <f>C4</f>
+        <v>1.7840000000000002E-2</v>
       </c>
       <c r="D21">
         <f t="shared" si="5"/>
-        <v>7.5132000000000001E-8</v>
+        <v>1.7840000000000003E-8</v>
       </c>
       <c r="E21">
         <v>96000</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="6"/>
-        <v>0.99281327689425547</v>
+        <v>0.99828882573100886</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1037,18 +1056,19 @@
       </c>
       <c r="C24" cm="1">
         <f t="array" ref="C24">SUM(B19:B22*C19:C22)</f>
-        <v>0.10029300000000001</v>
+        <v>3.1304999999999999E-2</v>
       </c>
       <c r="D24">
         <f t="shared" si="5"/>
-        <v>1.0029300000000001E-7</v>
+        <v>3.1305000000000001E-8</v>
       </c>
       <c r="E24">
-        <v>96000</v>
+        <f>0.2*E22</f>
+        <v>19200</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" ref="F24" si="7">EXP(-D24*E24)</f>
-        <v>0.99041807402582449</v>
+        <v>0.99939912459797264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>